<commit_message>
Signed-off-by: Risa Naka <rn96@cs.cornell.edu>
</commit_message>
<xml_diff>
--- a/2011_2012/Mar1Mar15Cycle/ssCalculation.xlsx
+++ b/2011_2012/Mar1Mar15Cycle/ssCalculation.xlsx
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD122" sqref="D2:AD122"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>